<commit_message>
fix the bug of p_grid_max method
</commit_message>
<xml_diff>
--- a/output/experiments/thesis_sensitivity/sensitive-bat-pv-minimize-cap.xlsx
+++ b/output/experiments/thesis_sensitivity/sensitive-bat-pv-minimize-cap.xlsx
@@ -5,25 +5,22 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lunlo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\Energy_grid_new\output\experiments\thesis_sensitivity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7654AE68-3941-4A7F-B37C-BDC59ACDB1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56841DB7-F828-4BF3-B033-717B3A41C404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$305</definedName>
-  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4251" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4252" uniqueCount="318">
   <si>
     <t>status</t>
   </si>
@@ -907,7 +904,7 @@
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-368.0-unconscious-10-01-11-01-Sum-ALL-Sum-minimize_cap-2023-09-06_009.xlsx</t>
   </si>
   <si>
-    <t>MPC-MPC-optimal-Prediction-unconscious-1.5-0.6-0.6-flex-368.0-unconscious-10-01-11-01-Sum-ALL-Sum-minimize_cap-2023-09-06_011.xlsx</t>
+    <t>MPC-MPC-optimal-Prediction-unconscious-1.5-0.6-0.6-flex-368.0-unconscious-10-01-11-01-Sum-ALL-Sum-minimize_cap-2023-09-06_012.xlsx</t>
   </si>
   <si>
     <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-368.0-unconscious-10-01-11-01-Sum-ALL-Sum-minimize_cap-2023-09-06_009.xlsx</t>
@@ -983,11 +980,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -995,8 +992,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1042,7 +1046,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1058,7 +1062,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1381,12 +1385,12 @@
   <dimension ref="A1:BD305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
@@ -1556,7 +1560,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1720,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1884,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2048,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2212,7 +2216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2376,7 +2380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2540,7 +2544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2704,7 +2708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2868,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3032,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3196,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3360,7 +3364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3524,7 +3528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3688,7 +3692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3852,7 +3856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4016,7 +4020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4180,7 +4184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4344,7 +4348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4508,7 +4512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4672,7 +4676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4836,7 +4840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5000,7 +5004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -5164,7 +5168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5328,7 +5332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5492,7 +5496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5656,7 +5660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5820,7 +5824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5984,7 +5988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -6148,7 +6152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -6312,7 +6316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -6476,7 +6480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -6640,7 +6644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -6804,7 +6808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -6968,7 +6972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -7132,7 +7136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -7296,7 +7300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -7460,7 +7464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -7624,7 +7628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -7788,7 +7792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -7952,7 +7956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -8116,7 +8120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -8280,7 +8284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -8444,7 +8448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -8608,7 +8612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -8772,7 +8776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -8936,7 +8940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -9100,7 +9104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -9264,7 +9268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -9428,7 +9432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -9592,7 +9596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -9756,7 +9760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -9920,7 +9924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -10084,7 +10088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -10248,7 +10252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -10412,7 +10416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -10576,7 +10580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -10740,7 +10744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -10904,7 +10908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -11068,7 +11072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -11232,7 +11236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -11396,7 +11400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -11560,7 +11564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -11724,7 +11728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -11888,7 +11892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -12052,7 +12056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -12216,7 +12220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -12380,7 +12384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -12544,7 +12548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -12708,7 +12712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -12872,7 +12876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -13036,7 +13040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -13200,7 +13204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -13364,7 +13368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -13528,7 +13532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -13692,7 +13696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -13856,7 +13860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -14020,7 +14024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -14184,7 +14188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -14348,7 +14352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -14512,7 +14516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -14676,7 +14680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -14840,7 +14844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -15004,7 +15008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -15168,7 +15172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -15332,7 +15336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -15496,7 +15500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -15660,7 +15664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -15824,7 +15828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -15988,7 +15992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -16152,7 +16156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -16316,7 +16320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -16480,7 +16484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -16644,7 +16648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -16808,7 +16812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -16972,7 +16976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -17136,7 +17140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -17300,7 +17304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -17464,7 +17468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -17628,7 +17632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -17792,7 +17796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -17956,7 +17960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -18120,7 +18124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -18284,7 +18288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -18448,7 +18452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -18612,7 +18616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -18776,7 +18780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -18940,7 +18944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -19104,7 +19108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -19268,7 +19272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -19432,7 +19436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -19497,7 +19501,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="112" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -19562,7 +19566,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="113" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -19627,7 +19631,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="114" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -19692,7 +19696,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="115" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -19757,7 +19761,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="116" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -19822,7 +19826,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="117" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -19887,7 +19891,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="118" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -19952,7 +19956,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="119" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -20017,7 +20021,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="120" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -20082,7 +20086,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="121" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -20147,7 +20151,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="122" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -20212,7 +20216,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="123" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -20277,7 +20281,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="124" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -20342,7 +20346,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="125" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -20407,7 +20411,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="126" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -20571,7 +20575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -20735,7 +20739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -20899,7 +20903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -21063,7 +21067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -21227,7 +21231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -21391,7 +21395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -21555,7 +21559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -21719,7 +21723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -21883,7 +21887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -22047,7 +22051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -22211,7 +22215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -22375,7 +22379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -22539,7 +22543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -22703,7 +22707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -22867,7 +22871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -23031,7 +23035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -23195,7 +23199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -23359,7 +23363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -23523,7 +23527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -23687,7 +23691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -23851,7 +23855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -24015,7 +24019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -24179,7 +24183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -24343,7 +24347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -24507,7 +24511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -24671,7 +24675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -24835,7 +24839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -24999,7 +25003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -25163,7 +25167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -25327,7 +25331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -25491,7 +25495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -25655,7 +25659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -25819,7 +25823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -25983,7 +25987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -26147,7 +26151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -26311,7 +26315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -26475,7 +26479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -26639,7 +26643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -26803,7 +26807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -26967,7 +26971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -27131,7 +27135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -27295,7 +27299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -27459,7 +27463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -27623,7 +27627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -27787,7 +27791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -27852,7 +27856,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="172" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -27917,7 +27921,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="173" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -27982,7 +27986,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="174" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -28047,7 +28051,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="175" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -28112,7 +28116,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="176" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -28177,7 +28181,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="177" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -28242,7 +28246,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="178" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -28307,7 +28311,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="179" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -28372,7 +28376,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="180" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -28437,7 +28441,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="181" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -28502,7 +28506,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="182" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -28567,7 +28571,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="183" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -28632,7 +28636,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="184" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -28697,7 +28701,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="185" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -28762,7 +28766,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="186" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -28926,7 +28930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -29090,7 +29094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -29254,7 +29258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -29418,7 +29422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -29582,7 +29586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -29746,7 +29750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -29910,7 +29914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -30074,7 +30078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -30238,7 +30242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -30402,7 +30406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -30566,7 +30570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -30730,7 +30734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -30894,7 +30898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -31058,7 +31062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -31222,7 +31226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -31386,7 +31390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -31550,7 +31554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -31714,7 +31718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -31878,7 +31882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -32042,7 +32046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -32206,7 +32210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>206</v>
       </c>
@@ -32370,7 +32374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -32534,7 +32538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>208</v>
       </c>
@@ -32698,7 +32702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -32862,7 +32866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>210</v>
       </c>
@@ -33026,7 +33030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>211</v>
       </c>
@@ -33190,7 +33194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>212</v>
       </c>
@@ -33354,7 +33358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>213</v>
       </c>
@@ -33518,7 +33522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>214</v>
       </c>
@@ -33682,7 +33686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -33846,7 +33850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>216</v>
       </c>
@@ -34010,7 +34014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -34174,7 +34178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>218</v>
       </c>
@@ -34338,7 +34342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>219</v>
       </c>
@@ -34502,7 +34506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>220</v>
       </c>
@@ -34666,7 +34670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>221</v>
       </c>
@@ -34830,7 +34834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>222</v>
       </c>
@@ -34994,7 +34998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>223</v>
       </c>
@@ -35158,7 +35162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>224</v>
       </c>
@@ -35322,7 +35326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>225</v>
       </c>
@@ -35486,7 +35490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>226</v>
       </c>
@@ -35650,7 +35654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>227</v>
       </c>
@@ -35814,7 +35818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>228</v>
       </c>
@@ -35978,7 +35982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>229</v>
       </c>
@@ -36142,7 +36146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>230</v>
       </c>
@@ -36207,7 +36211,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="232" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>231</v>
       </c>
@@ -36272,7 +36276,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="233" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>232</v>
       </c>
@@ -36337,7 +36341,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="234" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>233</v>
       </c>
@@ -36402,7 +36406,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="235" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>234</v>
       </c>
@@ -36467,7 +36471,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="236" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>235</v>
       </c>
@@ -36532,7 +36536,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="237" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>236</v>
       </c>
@@ -36597,7 +36601,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="238" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>237</v>
       </c>
@@ -36662,7 +36666,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="239" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>238</v>
       </c>
@@ -36727,7 +36731,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="240" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>239</v>
       </c>
@@ -36792,7 +36796,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="241" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>240</v>
       </c>
@@ -36857,7 +36861,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="242" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>241</v>
       </c>
@@ -36922,7 +36926,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="243" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>242</v>
       </c>
@@ -36987,7 +36991,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="244" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>243</v>
       </c>
@@ -37052,7 +37056,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="245" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>244</v>
       </c>
@@ -37117,7 +37121,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="246" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>245</v>
       </c>
@@ -37281,7 +37285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>246</v>
       </c>
@@ -37445,7 +37449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>247</v>
       </c>
@@ -37609,7 +37613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>248</v>
       </c>
@@ -37773,7 +37777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>249</v>
       </c>
@@ -37937,7 +37941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>250</v>
       </c>
@@ -38101,7 +38105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>251</v>
       </c>
@@ -38265,7 +38269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>252</v>
       </c>
@@ -38429,7 +38433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>253</v>
       </c>
@@ -38593,7 +38597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>254</v>
       </c>
@@ -38757,7 +38761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>255</v>
       </c>
@@ -38921,7 +38925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>256</v>
       </c>
@@ -39085,7 +39089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>257</v>
       </c>
@@ -39249,7 +39253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>258</v>
       </c>
@@ -39413,7 +39417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>259</v>
       </c>
@@ -39577,7 +39581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>260</v>
       </c>
@@ -39741,7 +39745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>261</v>
       </c>
@@ -39905,7 +39909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>262</v>
       </c>
@@ -40069,7 +40073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>263</v>
       </c>
@@ -40233,7 +40237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>264</v>
       </c>
@@ -40397,7 +40401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>265</v>
       </c>
@@ -40561,12 +40565,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>266</v>
       </c>
-      <c r="B267">
-        <v>0</v>
+      <c r="B267" t="s">
+        <v>56</v>
       </c>
       <c r="C267" t="s">
         <v>58</v>
@@ -40625,11 +40629,107 @@
       <c r="U267" t="s">
         <v>73</v>
       </c>
+      <c r="V267">
+        <v>382.82612488587972</v>
+      </c>
+      <c r="W267">
+        <v>30.989583333333329</v>
+      </c>
+      <c r="X267">
+        <v>1118.8134438283739</v>
+      </c>
       <c r="Y267" t="s">
         <v>294</v>
       </c>
+      <c r="Z267">
+        <v>382.82612488587972</v>
+      </c>
+      <c r="AA267">
+        <v>367.70283721464682</v>
+      </c>
+      <c r="AB267">
+        <v>15.12328767123288</v>
+      </c>
+      <c r="AC267">
+        <v>15.12328767123288</v>
+      </c>
+      <c r="AD267">
+        <v>368</v>
+      </c>
+      <c r="AE267">
+        <v>4.7451656713307502</v>
+      </c>
+      <c r="AF267">
+        <v>0</v>
+      </c>
+      <c r="AG267">
+        <v>0</v>
+      </c>
+      <c r="AH267">
+        <v>0.142140296910235</v>
+      </c>
+      <c r="AI267">
+        <v>0.142140296910235</v>
+      </c>
+      <c r="AJ267">
+        <v>0.13652514041983421</v>
+      </c>
+      <c r="AL267">
+        <v>116.4712629</v>
+      </c>
+      <c r="AM267">
+        <v>251.23157431464679</v>
+      </c>
+      <c r="AO267">
+        <v>91.740504201680679</v>
+      </c>
+      <c r="AP267">
+        <v>1861.262727529411</v>
+      </c>
+      <c r="AQ267">
+        <v>832.03490310410029</v>
+      </c>
+      <c r="AR267">
+        <v>2693.2976306335108</v>
+      </c>
+      <c r="AS267">
+        <v>932.82719817364341</v>
+      </c>
+      <c r="AT267">
+        <v>1793.217362061135</v>
+      </c>
+      <c r="AU267">
+        <v>9.3296772894541462</v>
+      </c>
+      <c r="AV267">
+        <v>252.35062875097921</v>
+      </c>
+      <c r="AW267">
+        <v>1.11905443633237</v>
+      </c>
+      <c r="AX267">
+        <v>194.11877150000001</v>
+      </c>
+      <c r="AY267">
+        <v>0</v>
+      </c>
+      <c r="AZ267">
+        <v>0</v>
+      </c>
+      <c r="BA267">
+        <v>-8.4512329000000008</v>
+      </c>
+      <c r="BB267">
+        <v>25.231371499999991</v>
+      </c>
+      <c r="BC267">
+        <v>0</v>
+      </c>
+      <c r="BD267">
+        <v>0</v>
+      </c>
     </row>
-    <row r="268" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>267</v>
       </c>
@@ -40793,7 +40893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>268</v>
       </c>
@@ -40957,7 +41057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>269</v>
       </c>
@@ -41121,7 +41221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>270</v>
       </c>
@@ -41285,7 +41385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>271</v>
       </c>
@@ -41449,7 +41549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>272</v>
       </c>
@@ -41613,7 +41713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>273</v>
       </c>
@@ -41777,7 +41877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>274</v>
       </c>
@@ -41941,7 +42041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>275</v>
       </c>
@@ -42105,7 +42205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>276</v>
       </c>
@@ -42269,7 +42369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>277</v>
       </c>
@@ -42433,7 +42533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>278</v>
       </c>
@@ -42597,7 +42697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>279</v>
       </c>
@@ -42761,7 +42861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>280</v>
       </c>
@@ -42925,7 +43025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>281</v>
       </c>
@@ -43089,7 +43189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>282</v>
       </c>
@@ -43253,7 +43353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="284" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>283</v>
       </c>
@@ -43417,7 +43517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="285" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>284</v>
       </c>
@@ -43581,7 +43681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>285</v>
       </c>
@@ -43745,7 +43845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>286</v>
       </c>
@@ -43909,7 +44009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>287</v>
       </c>
@@ -44073,7 +44173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>288</v>
       </c>
@@ -44237,7 +44337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>289</v>
       </c>
@@ -44401,7 +44501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>290</v>
       </c>
@@ -44466,7 +44566,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="292" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>291</v>
       </c>
@@ -44531,7 +44631,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="293" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>292</v>
       </c>
@@ -44596,7 +44696,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="294" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>293</v>
       </c>
@@ -44661,7 +44761,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="295" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>294</v>
       </c>
@@ -44726,7 +44826,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="296" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>295</v>
       </c>
@@ -44791,7 +44891,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="297" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>296</v>
       </c>
@@ -44856,7 +44956,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="298" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>297</v>
       </c>
@@ -44921,7 +45021,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="299" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>298</v>
       </c>
@@ -44986,7 +45086,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="300" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>299</v>
       </c>
@@ -45051,7 +45151,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="301" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>300</v>
       </c>
@@ -45116,7 +45216,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="302" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>301</v>
       </c>
@@ -45181,7 +45281,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="303" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>302</v>
       </c>
@@ -45246,7 +45346,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="304" spans="1:56" x14ac:dyDescent="0.45">
+    <row r="304" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>303</v>
       </c>
@@ -45311,7 +45411,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="305" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>304</v>
       </c>
@@ -45377,6 +45477,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>